<commit_message>
saving work, need to retool testing suite
</commit_message>
<xml_diff>
--- a/tests/test_data/test_pipeline_progress.xlsx
+++ b/tests/test_data/test_pipeline_progress.xlsx
@@ -64,16 +64,16 @@
     <t xml:space="preserve">prefix|Emissions|BC|setcor2|Harmonized-DB</t>
   </si>
   <si>
+    <t xml:space="preserve">prefix|Emissions|Sulfur|Harmonized-DB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mt SO2/yr</t>
+  </si>
+  <si>
     <t xml:space="preserve">prefix|Emissions|OC|Harmonized-DB</t>
   </si>
   <si>
     <t xml:space="preserve">Mt OC/yr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prefix|Emissions|Sulfur|Harmonized-DB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mt SO2/yr</t>
   </si>
   <si>
     <t xml:space="preserve">regiona</t>
@@ -170,13 +170,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -196,10 +200,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -301,7 +305,7 @@
         <v>17.1428571428571</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>7</v>
       </c>
@@ -314,17 +318,17 @@
       <c r="D5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>31.4285714285714</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F5" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>17.1428571428571</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>7</v>
       </c>
@@ -337,17 +341,18 @@
       <c r="D6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="0" t="n">
-        <v>15</v>
+      <c r="F6" s="2" t="n">
+        <f aca="false">SUM(F7:F8)</f>
+        <v>35</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>17.1428571428571</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>7</v>
       </c>
@@ -360,18 +365,18 @@
       <c r="D7" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="0" t="n">
-        <v>10</v>
+      <c r="F7" s="2" t="n">
+        <v>15</v>
       </c>
       <c r="G7" s="0" t="n">
         <f aca="false">G6*F7/F6</f>
-        <v>11.4285714285714</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7.34693877551021</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>7</v>
       </c>
@@ -384,17 +389,25 @@
       <c r="D8" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="0" t="n">
-        <v>5</v>
+      <c r="F8" s="2" t="n">
+        <v>20</v>
       </c>
       <c r="G8" s="0" t="n">
         <f aca="false">G6-G7</f>
-        <v>5.71428571428572</v>
-      </c>
-    </row>
+        <v>9.79591836734694</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>